<commit_message>
Adicionado imagem do projeto
</commit_message>
<xml_diff>
--- a/Projeto 1.xlsx
+++ b/Projeto 1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psolr\Documents\Edu\Pessoal\Curso Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psolr\Desktop\Projetos pessoais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A8154F-9F18-4534-8564-08602F466ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A5F383-4F08-4543-B3BB-1F67544152A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,8 +156,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="165" formatCode="0.000%"/>
-    <numFmt numFmtId="167" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -648,95 +648,35 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
     </xf>
     <xf numFmtId="10" fontId="6" fillId="7" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
     </xf>
     <xf numFmtId="8" fontId="8" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
     </xf>
     <xf numFmtId="8" fontId="8" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -788,22 +728,82 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="9" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutro" xfId="2" builtinId="28"/>
@@ -864,6 +864,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-B909-4C8A-931A-56C6B845C70C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -879,6 +884,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-B909-4C8A-931A-56C6B845C70C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -894,6 +904,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-B909-4C8A-931A-56C6B845C70C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -909,6 +924,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-B909-4C8A-931A-56C6B845C70C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -924,6 +944,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-B909-4C8A-931A-56C6B845C70C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -939,6 +964,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-B909-4C8A-931A-56C6B845C70C}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -2030,110 +2060,110 @@
     <row r="6" spans="2:4" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:4" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="55"/>
     </row>
     <row r="9" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16">
+      <c r="C9" s="57"/>
+      <c r="D9" s="8">
         <v>2000</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19">
+      <c r="C10" s="59"/>
+      <c r="D10" s="9">
         <v>8.8999999999999999E-3</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22">
+      <c r="C11" s="61"/>
+      <c r="D11" s="10">
         <f>D9*30%</f>
         <v>600</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="64"/>
     </row>
     <row r="14" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25">
+      <c r="C14" s="66"/>
+      <c r="D14" s="11">
         <v>600</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="28">
+      <c r="C15" s="68"/>
+      <c r="D15" s="12">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="29">
+      <c r="C16" s="68"/>
+      <c r="D16" s="13">
         <v>1.0789999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32">
+      <c r="C17" s="50"/>
+      <c r="D17" s="14">
         <f>FV(taxa_mensal,qtd_anos*12,aporte*-1)</f>
         <v>145970.52751810331</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="35">
+      <c r="C18" s="52"/>
+      <c r="D18" s="15">
         <f>patrimonio*$D$10</f>
         <v>1299.1376949111195</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="11"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" ht="30.75" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="47" t="s">
+      <c r="C20" s="7"/>
+      <c r="D20" s="27" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2141,14 +2171,14 @@
       <c r="A21" s="2">
         <v>2</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="37">
+      <c r="C21" s="17">
         <f>FV($D$16,A21*12,$D$14*-1)</f>
         <v>16336.57637858713</v>
       </c>
-      <c r="D21" s="38">
+      <c r="D21" s="18">
         <f>C21*rendimento_carteira</f>
         <v>145.39552976942545</v>
       </c>
@@ -2157,14 +2187,14 @@
       <c r="A22" s="2">
         <v>5</v>
       </c>
-      <c r="B22" s="39" t="s">
+      <c r="B22" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="40">
+      <c r="C22" s="20">
         <f>FV($D$16,A22*12,$D$14*-1)</f>
         <v>50266.148399092584</v>
       </c>
-      <c r="D22" s="41">
+      <c r="D22" s="21">
         <f>C22*rendimento_carteira</f>
         <v>447.368720751924</v>
       </c>
@@ -2173,14 +2203,14 @@
       <c r="A23" s="2">
         <v>10</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="40">
+      <c r="C23" s="20">
         <f>FV($D$16,A23*12,$D$14*-1)</f>
         <v>145970.52751810331</v>
       </c>
-      <c r="D23" s="41">
+      <c r="D23" s="21">
         <f>C23*rendimento_carteira</f>
         <v>1299.1376949111195</v>
       </c>
@@ -2189,14 +2219,14 @@
       <c r="A24" s="2">
         <v>20</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="40">
+      <c r="C24" s="20">
         <f>FV($D$16,A24*12,$D$14*-1)</f>
         <v>675119.04005824833</v>
       </c>
-      <c r="D24" s="41">
+      <c r="D24" s="21">
         <f>C24*rendimento_carteira</f>
         <v>6008.5594565184101</v>
       </c>
@@ -2205,14 +2235,14 @@
       <c r="A25" s="2">
         <v>30</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="43">
+      <c r="C25" s="23">
         <f>FV($D$16,A25*12,$D$14*-1)</f>
         <v>2593301.7930028285</v>
       </c>
-      <c r="D25" s="44">
+      <c r="D25" s="24">
         <f>C25*rendimento_carteira</f>
         <v>23080.385957725175</v>
       </c>
@@ -2220,13 +2250,13 @@
     <row r="26" spans="1:4" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="46" t="s">
+      <c r="C28" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="46"/>
+      <c r="D28" s="26"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
@@ -2239,98 +2269,98 @@
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="54" t="s">
+      <c r="B31" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="55" t="s">
+      <c r="C31" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="56" t="s">
+      <c r="D31" s="36" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="60" t="s">
+      <c r="B32" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="61">
+      <c r="C32" s="41">
         <f>VLOOKUP($C$28&amp;"-"&amp;B32,Planilha1!$A:$D,4,FALSE)</f>
         <v>0.32</v>
       </c>
-      <c r="D32" s="62">
+      <c r="D32" s="42">
         <f>C32*$C$29</f>
         <v>192</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="63" t="s">
+      <c r="B33" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="64">
+      <c r="C33" s="44">
         <f>VLOOKUP($C$28&amp;"-"&amp;B33,Planilha1!$A:$D,4,FALSE)</f>
         <v>0.35</v>
       </c>
-      <c r="D33" s="65">
+      <c r="D33" s="45">
         <f t="shared" ref="D33:D37" si="0">C33*$C$29</f>
         <v>210</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="63" t="s">
+      <c r="B34" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="64">
+      <c r="C34" s="44">
         <f>VLOOKUP($C$28&amp;"-"&amp;B34,Planilha1!$A:$D,4,FALSE)</f>
         <v>0.08</v>
       </c>
-      <c r="D34" s="65">
+      <c r="D34" s="45">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="63" t="s">
+      <c r="B35" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="64">
+      <c r="C35" s="44">
         <f>VLOOKUP($C$28&amp;"-"&amp;B35,Planilha1!$A:$D,4,FALSE)</f>
         <v>0.05</v>
       </c>
-      <c r="D35" s="65">
+      <c r="D35" s="45">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="63" t="s">
+      <c r="B36" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="64">
+      <c r="C36" s="44">
         <f>VLOOKUP($C$28&amp;"-"&amp;B36,Planilha1!$A:$D,4,FALSE)</f>
         <v>0.1</v>
       </c>
-      <c r="D36" s="65">
+      <c r="D36" s="45">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="66" t="s">
+      <c r="B37" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="67">
+      <c r="C37" s="47">
         <f>VLOOKUP($C$28&amp;"-"&amp;B37,Planilha1!$A:$D,4,FALSE)</f>
         <v>0.1</v>
       </c>
-      <c r="D37" s="68">
+      <c r="D37" s="48">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="57"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="59">
+      <c r="B38" s="37"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="39">
         <f>SUM(D32:D37)</f>
         <v>600</v>
       </c>
@@ -2401,7 +2431,7 @@
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="33" t="s">
         <v>28</v>
       </c>
       <c r="D2" t="s">
@@ -2419,7 +2449,7 @@
       <c r="C3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="28">
         <v>0.3</v>
       </c>
     </row>
@@ -2434,7 +2464,7 @@
       <c r="C4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="28">
         <v>0.5</v>
       </c>
     </row>
@@ -2449,7 +2479,7 @@
       <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="28">
         <v>0.1</v>
       </c>
     </row>
@@ -2464,7 +2494,7 @@
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="28">
         <v>0.1</v>
       </c>
     </row>
@@ -2479,22 +2509,22 @@
       <c r="C7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="49" t="str">
+      <c r="A8" s="29" t="str">
         <f t="shared" si="0"/>
         <v>Conservador-HOTELARIA</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="51">
+      <c r="D8" s="31">
         <v>0</v>
       </c>
     </row>
@@ -2509,7 +2539,7 @@
       <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="48">
+      <c r="D9" s="28">
         <v>0.32</v>
       </c>
     </row>
@@ -2524,7 +2554,7 @@
       <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="48">
+      <c r="D10" s="28">
         <v>0.35</v>
       </c>
     </row>
@@ -2539,7 +2569,7 @@
       <c r="C11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="48">
+      <c r="D11" s="28">
         <v>0.08</v>
       </c>
     </row>
@@ -2554,7 +2584,7 @@
       <c r="C12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="48">
+      <c r="D12" s="28">
         <v>0.05</v>
       </c>
     </row>
@@ -2569,22 +2599,22 @@
       <c r="C13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="28">
         <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49" t="str">
+      <c r="A14" s="29" t="str">
         <f t="shared" si="0"/>
         <v>Moderado-HOTELARIA</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="50" t="s">
+      <c r="C14" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="51">
+      <c r="D14" s="31">
         <v>0.1</v>
       </c>
     </row>
@@ -2593,13 +2623,13 @@
         <f t="shared" si="0"/>
         <v>Agressivo-PAPEL</v>
       </c>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="32" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D15" s="28">
         <v>0.5</v>
       </c>
     </row>
@@ -2608,13 +2638,13 @@
         <f t="shared" si="0"/>
         <v>Agressivo-TIJOLO</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="32" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="28">
         <v>0.1</v>
       </c>
     </row>
@@ -2623,13 +2653,13 @@
         <f t="shared" si="0"/>
         <v>Agressivo-HÍBRIDOS</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="32" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D17" s="28">
         <v>0.05</v>
       </c>
     </row>
@@ -2638,13 +2668,13 @@
         <f t="shared" si="0"/>
         <v>Agressivo-FOF'S</v>
       </c>
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="32" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="48">
+      <c r="D18" s="28">
         <v>0.05</v>
       </c>
     </row>
@@ -2653,13 +2683,13 @@
         <f t="shared" si="0"/>
         <v>Agressivo-DESENVOLVIMENTO</v>
       </c>
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="32" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="48">
+      <c r="D19" s="28">
         <v>0.2</v>
       </c>
     </row>
@@ -2668,13 +2698,13 @@
         <f t="shared" si="0"/>
         <v>Agressivo-HOTELARIA</v>
       </c>
-      <c r="B20" s="52" t="s">
+      <c r="B20" s="32" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="48">
+      <c r="D20" s="28">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>